<commit_message>
new from Sep.2022 BP
</commit_message>
<xml_diff>
--- a/tables-pt/listaiban.xlsx
+++ b/tables-pt/listaiban.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="379">
   <si>
     <t>0001</t>
   </si>
@@ -288,9 +288,6 @@
     <t>BANCO DE INVESTIMENTO GLOBAL, SA</t>
   </si>
   <si>
-    <t>BANCO SANTANDER CONSUMER PORTUGAL, SA</t>
-  </si>
-  <si>
     <t>MONTEPIO INVESTIMENTO, SA</t>
   </si>
   <si>
@@ -319,9 +316,6 @@
   </si>
   <si>
     <t>VOLKSWAGEN BANK GMBH - SUCURSAL EM PORTUGAL</t>
-  </si>
-  <si>
-    <t>BANK OF CHINA (LUXEMBOURG), SA LISBON BRANCH - SUCURSAL EM PORTUGAL</t>
   </si>
   <si>
     <t>CREDIT SUISSE (LUXEMBOURG), SA - SUCURSAL EM PORTUGAL</t>
@@ -401,9 +395,6 @@
     <t>8706</t>
   </si>
   <si>
-    <t>OREY FINANCIAL - INSTITUICAO FINANCEIRA DE CREDITO, SA</t>
-  </si>
-  <si>
     <t>0191</t>
   </si>
   <si>
@@ -853,9 +844,6 @@
   </si>
   <si>
     <t>SOFID - SOCIEDADE PARA O FINANCIAMENTO DO DESENVOLVIMENTO, INSTITUIÇÃO FINANCEIRA DE CRÉDITO, SA</t>
-  </si>
-  <si>
-    <t>FCA CAPITAL PORTUGAL, INSTITUIÇÃO FINANCEIRA DE CRÉDITO, SA</t>
   </si>
   <si>
     <t>0848</t>
@@ -1243,6 +1231,31 @@
   </si>
   <si>
     <t>Sucursais de Instituições de Pagamento com Sede na U.E.</t>
+  </si>
+  <si>
+    <t>SANTANDER CONSUMER FINANCE, S.A. - SUCURSAL EM PORTUGAL</t>
+  </si>
+  <si>
+    <t>BANK OF CHINA (EUROPE), SA LISBON BRANCH - SUCURSAL EM PORTUGAL</t>
+  </si>
+  <si>
+    <t>FCA BANK S.P.A. - SUCURSAL EM PORTUGAL</t>
+  </si>
+  <si>
+    <t>5845</t>
+  </si>
+  <si>
+    <t>UNIFIEDPOST PAYMENTS S.A. - SUCURSAL EM
+PORTUGAL</t>
+  </si>
+  <si>
+    <t>7501</t>
+  </si>
+  <si>
+    <t>MARTRUST EUROPE, S.A.</t>
+  </si>
+  <si>
+    <t>OREY FINANCIAL - INSTITUIÇÃO FINANCEIRA DE CRÉDITO, SA</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1772,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="254" name="ListaIBAN1" displayName="ListaIBAN1" ref="A1:D176" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:D176"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="254" name="ListaIBAN1" displayName="ListaIBAN1" ref="A1:D178" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:D178"/>
   <sortState ref="A2:H193">
     <sortCondition ref="A2:A193"/>
     <sortCondition ref="B2:B193"/>
@@ -2062,18 +2075,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D239"/>
+  <dimension ref="A1:D241"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A181" sqref="A181:D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.42578125" style="3" customWidth="1"/>
+    <col min="1" max="2" width="45" style="3" customWidth="1"/>
     <col min="3" max="3" width="124" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="6.42578125" style="3"/>
@@ -2081,16 +2094,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="8" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2104,7 +2117,7 @@
         <v>73</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2115,10 +2128,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2129,10 +2142,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2146,7 +2159,7 @@
         <v>74</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2160,7 +2173,7 @@
         <v>75</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2174,7 +2187,7 @@
         <v>76</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2188,7 +2201,7 @@
         <v>77</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2199,10 +2212,10 @@
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2216,7 +2229,7 @@
         <v>78</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2230,7 +2243,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2244,7 +2257,7 @@
         <v>80</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,10 +2268,10 @@
         <v>11</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>236</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2269,10 +2282,10 @@
         <v>12</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2286,7 +2299,7 @@
         <v>71</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2297,10 +2310,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2311,10 +2324,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2328,7 +2341,7 @@
         <v>81</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2336,13 +2349,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2350,13 +2363,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2364,13 +2377,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2378,13 +2391,13 @@
         <v>17</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2392,13 +2405,13 @@
         <v>17</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2406,13 +2419,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2420,13 +2433,13 @@
         <v>17</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2434,13 +2447,13 @@
         <v>17</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2448,13 +2461,13 @@
         <v>17</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2462,13 +2475,13 @@
         <v>17</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2476,13 +2489,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2490,13 +2503,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2504,13 +2517,13 @@
         <v>17</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2518,13 +2531,13 @@
         <v>17</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2532,13 +2545,13 @@
         <v>17</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D33" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2546,13 +2559,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2560,13 +2573,13 @@
         <v>17</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2574,13 +2587,13 @@
         <v>17</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2588,13 +2601,13 @@
         <v>17</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2602,13 +2615,13 @@
         <v>17</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2616,13 +2629,13 @@
         <v>17</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2630,13 +2643,13 @@
         <v>17</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2644,13 +2657,13 @@
         <v>17</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2658,13 +2671,13 @@
         <v>17</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2672,13 +2685,13 @@
         <v>17</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2686,13 +2699,13 @@
         <v>17</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2700,13 +2713,13 @@
         <v>17</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2714,13 +2727,13 @@
         <v>17</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2728,13 +2741,13 @@
         <v>17</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2742,13 +2755,13 @@
         <v>17</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2756,13 +2769,13 @@
         <v>17</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2770,13 +2783,13 @@
         <v>17</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2784,13 +2797,13 @@
         <v>17</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2798,13 +2811,13 @@
         <v>17</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2812,13 +2825,13 @@
         <v>17</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2826,13 +2839,13 @@
         <v>17</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2840,13 +2853,13 @@
         <v>17</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,13 +2867,13 @@
         <v>17</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2868,13 +2881,13 @@
         <v>17</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2882,13 +2895,13 @@
         <v>17</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2896,13 +2909,13 @@
         <v>17</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2910,13 +2923,13 @@
         <v>17</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2924,13 +2937,13 @@
         <v>17</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2938,13 +2951,13 @@
         <v>17</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2952,13 +2965,13 @@
         <v>17</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2966,13 +2979,13 @@
         <v>17</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,13 +2993,13 @@
         <v>17</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D65" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2994,13 +3007,13 @@
         <v>17</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3008,13 +3021,13 @@
         <v>17</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3022,13 +3035,13 @@
         <v>17</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D68" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3036,13 +3049,13 @@
         <v>17</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D69" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3050,13 +3063,13 @@
         <v>17</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3064,13 +3077,13 @@
         <v>17</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D71" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3078,13 +3091,13 @@
         <v>17</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3092,13 +3105,13 @@
         <v>17</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3106,13 +3119,13 @@
         <v>17</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3120,13 +3133,13 @@
         <v>17</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3134,13 +3147,13 @@
         <v>17</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3148,13 +3161,13 @@
         <v>17</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3162,13 +3175,13 @@
         <v>17</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3176,13 +3189,13 @@
         <v>17</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3190,13 +3203,13 @@
         <v>17</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3204,13 +3217,13 @@
         <v>17</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="82" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3218,13 +3231,13 @@
         <v>17</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3232,13 +3245,13 @@
         <v>17</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3246,13 +3259,13 @@
         <v>17</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3260,13 +3273,13 @@
         <v>17</v>
       </c>
       <c r="B85" s="23" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D85" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3274,13 +3287,13 @@
         <v>17</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3288,13 +3301,13 @@
         <v>17</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3302,13 +3315,13 @@
         <v>17</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D88" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3316,13 +3329,13 @@
         <v>17</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D89" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3330,13 +3343,13 @@
         <v>17</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3344,13 +3357,13 @@
         <v>17</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3358,13 +3371,13 @@
         <v>17</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3372,13 +3385,13 @@
         <v>17</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3386,13 +3399,13 @@
         <v>17</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3403,10 +3416,10 @@
         <v>18</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3420,7 +3433,7 @@
         <v>82</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -3431,10 +3444,10 @@
         <v>20</v>
       </c>
       <c r="C97" s="23" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D97" s="24" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3445,10 +3458,10 @@
         <v>21</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3462,7 +3475,7 @@
         <v>83</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3476,7 +3489,7 @@
         <v>84</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3487,10 +3500,10 @@
         <v>24</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3501,10 +3514,10 @@
         <v>25</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3515,10 +3528,10 @@
         <v>26</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3529,10 +3542,10 @@
         <v>27</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>85</v>
+        <v>371</v>
       </c>
       <c r="D104" s="12" t="s">
-        <v>103</v>
+        <v>236</v>
       </c>
     </row>
     <row r="105" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3543,10 +3556,10 @@
         <v>28</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D105" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="106" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3557,10 +3570,10 @@
         <v>29</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3571,10 +3584,10 @@
         <v>30</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3585,10 +3598,10 @@
         <v>31</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3599,10 +3612,10 @@
         <v>32</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3613,10 +3626,10 @@
         <v>33</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3627,10 +3640,10 @@
         <v>34</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3641,10 +3654,10 @@
         <v>35</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D112" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3655,10 +3668,10 @@
         <v>36</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3669,10 +3682,10 @@
         <v>37</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3683,10 +3696,10 @@
         <v>38</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3697,10 +3710,10 @@
         <v>39</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3711,52 +3724,52 @@
         <v>40</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D117" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="118" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B120" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3767,10 +3780,10 @@
         <v>41</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D121" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="122" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3781,10 +3794,10 @@
         <v>42</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3795,10 +3808,10 @@
         <v>43</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="124" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3809,10 +3822,10 @@
         <v>44</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3823,10 +3836,10 @@
         <v>45</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D125" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="126" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3837,10 +3850,10 @@
         <v>46</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3851,10 +3864,10 @@
         <v>47</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>96</v>
+        <v>372</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3865,150 +3878,150 @@
         <v>48</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="129" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="132" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B133" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D133" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B135" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C135" s="23" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D135" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="136" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="137" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="138" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="22" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D138" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="139" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4019,10 +4032,10 @@
         <v>49</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="140" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4033,10 +4046,10 @@
         <v>50</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4047,10 +4060,10 @@
         <v>51</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4061,10 +4074,10 @@
         <v>52</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D142" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="143" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4075,24 +4088,24 @@
         <v>53</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="144" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B144" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D144" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="145" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4103,10 +4116,10 @@
         <v>54</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>261</v>
-      </c>
-      <c r="D145" s="24" t="s">
-        <v>243</v>
+        <v>373</v>
+      </c>
+      <c r="D145" s="21" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="146" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4117,10 +4130,10 @@
         <v>55</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="147" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4131,10 +4144,10 @@
         <v>56</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="148" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4145,10 +4158,10 @@
         <v>57</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D148" s="12" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="149" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4159,38 +4172,38 @@
         <v>58</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D149" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="150" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D150" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B151" s="20" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C151" s="20" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D151" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="152" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4201,10 +4214,10 @@
         <v>59</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="153" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4215,10 +4228,10 @@
         <v>60</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="154" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4232,7 +4245,7 @@
         <v>72</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="155" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4243,10 +4256,10 @@
         <v>62</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>114</v>
+        <v>378</v>
       </c>
       <c r="D155" s="24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="156" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4257,10 +4270,10 @@
         <v>63</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D156" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="157" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4271,10 +4284,10 @@
         <v>64</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D157" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4285,353 +4298,386 @@
         <v>65</v>
       </c>
       <c r="C158" s="23" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D158" s="24" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="159" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C159" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="D159" s="21" t="s">
         <v>370</v>
-      </c>
-      <c r="D159" s="21" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="160" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="20" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B160" s="22" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D160" s="21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="20" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C161" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="D161" s="12" t="s">
-        <v>245</v>
+      <c r="B161" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="C161" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="D161" s="21" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="162" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="B162" s="13" t="s">
-        <v>246</v>
+      <c r="A162" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>121</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>247</v>
+        <v>367</v>
       </c>
       <c r="D162" s="12" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="20" t="s">
-        <v>365</v>
-      </c>
-      <c r="B163" s="22" t="s">
-        <v>365</v>
-      </c>
-      <c r="C163" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="D163" s="21" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B164" s="11" t="s">
-        <v>66</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="C163" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="D163" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B164" s="13" t="s">
+        <v>243</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="D164" s="12" t="s">
-        <v>104</v>
+        <v>363</v>
       </c>
     </row>
     <row r="165" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B165" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>268</v>
-      </c>
-      <c r="D165" s="12" t="s">
-        <v>244</v>
+      <c r="A165" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B165" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="C165" s="20" t="s">
+        <v>362</v>
+      </c>
+      <c r="D165" s="21" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="166" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C166" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D166" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C167" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D167" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B166" s="11" t="s">
+      <c r="B168" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C166" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D166" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="20" t="s">
+      <c r="C168" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D168" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B167" s="22" t="s">
+      <c r="B169" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C167" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D167" s="21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B168" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C168" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="D168" s="12" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C169" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="D169" s="12" t="s">
-        <v>244</v>
+      <c r="C169" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D169" s="21" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>118</v>
+        <v>232</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="171" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="172" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>271</v>
+        <v>115</v>
       </c>
       <c r="D172" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="173" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>207</v>
+        <v>116</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
       <c r="D173" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="174" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
-        <v>214</v>
+        <v>120</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C174" s="14" t="s">
-        <v>250</v>
+        <v>120</v>
+      </c>
+      <c r="C174" s="11" t="s">
+        <v>267</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="175" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="26" t="s">
+      <c r="A175" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B175" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D175" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B176" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C176" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D176" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B175" s="23" t="s">
+      <c r="B177" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C175" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="D175" s="24" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B176" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C176" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="D176" s="12" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A179" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B179" s="27"/>
-      <c r="C179" s="27"/>
-      <c r="D179" s="27"/>
-    </row>
-    <row r="180" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B180" s="28"/>
-      <c r="C180" s="28"/>
-      <c r="D180" s="28"/>
-    </row>
-    <row r="181" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A181" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B181" s="28"/>
-      <c r="C181" s="28"/>
-      <c r="D181" s="28"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="5"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="5"/>
-      <c r="D182" s="5"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B183" s="5"/>
-      <c r="C183" s="5"/>
-      <c r="D183" s="5"/>
+      <c r="C177" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D177" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B178" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C178" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D178" s="12" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B181" s="27"/>
+      <c r="C181" s="27"/>
+      <c r="D181" s="27"/>
+    </row>
+    <row r="182" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A182" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B182" s="28"/>
+      <c r="C182" s="28"/>
+      <c r="D182" s="28"/>
+    </row>
+    <row r="183" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A183" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B183" s="28"/>
+      <c r="C183" s="28"/>
+      <c r="D183" s="28"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>110</v>
-      </c>
+      <c r="A184" s="5"/>
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
-        <v>111</v>
+      <c r="A185" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="5"/>
+      <c r="A186" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="6" t="s">
-        <v>112</v>
+      <c r="A187" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="2">
-        <v>44503</v>
-      </c>
+      <c r="A188" s="5"/>
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="4"/>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="4"/>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B189" s="5"/>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>44805</v>
+      </c>
+      <c r="B190" s="5"/>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="4"/>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A179:D179"/>
-    <mergeCell ref="A180:D180"/>
     <mergeCell ref="A181:D181"/>
+    <mergeCell ref="A182:D182"/>
+    <mergeCell ref="A183:D183"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4914,17 +4960,10 @@
 </file>
 
 <file path=customXml/itemProps10.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0201864C-B9C9-4D5A-BA22-67EC7A2D34AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A70DCD46-4906-4067-8163-C701F32689F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>